<commit_message>
Add SPI and SPI flash, small fixups
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="97">
   <si>
     <t xml:space="preserve">Pin name</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve">TIM2_CH1_ETR/JTDI/SPI1_NSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPI_CS</t>
   </si>
   <si>
     <t xml:space="preserve">PB0</t>
@@ -454,7 +457,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -660,148 +663,151 @@
       <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>20</v>
@@ -809,7 +815,7 @@
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>23</v>
@@ -817,64 +823,64 @@
     </row>
     <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync PWM/Servo and timers
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
   <si>
     <t xml:space="preserve">Pin name</t>
   </si>
@@ -62,6 +62,9 @@
     <t xml:space="preserve">USART2_RTS/ADC12_IN1/TIM2_CH2</t>
   </si>
   <si>
+    <t xml:space="preserve">AUDIO OUT?</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA2</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
     <t xml:space="preserve">SPI1_SCK/ADC12_IN5</t>
   </si>
   <si>
+    <t xml:space="preserve">FLASH SPI SCK</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA6</t>
   </si>
   <si>
@@ -95,6 +101,9 @@
     <t xml:space="preserve">TIM1_BKIN</t>
   </si>
   <si>
+    <t xml:space="preserve">FLASH SPI MISO</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA7</t>
   </si>
   <si>
@@ -104,6 +113,9 @@
     <t xml:space="preserve">TIM1_CH1N</t>
   </si>
   <si>
+    <t xml:space="preserve">FLASH SPI MOSI</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA8</t>
   </si>
   <si>
@@ -116,12 +128,18 @@
     <t xml:space="preserve">USART1_TX/TIM1_CH2</t>
   </si>
   <si>
+    <t xml:space="preserve">UART TX</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA10</t>
   </si>
   <si>
     <t xml:space="preserve">USART1_RX/TIM1_CH3</t>
   </si>
   <si>
+    <t xml:space="preserve">UART RX</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA11</t>
   </si>
   <si>
@@ -170,7 +188,7 @@
     <t xml:space="preserve">TIM2_CH1_ETR/JTDI/SPI1_NSS</t>
   </si>
   <si>
-    <t xml:space="preserve">SPI_CS</t>
+    <t xml:space="preserve">FLASH SPI CS</t>
   </si>
   <si>
     <t xml:space="preserve">PB0</t>
@@ -182,6 +200,9 @@
     <t xml:space="preserve">TIM1_CH2N</t>
   </si>
   <si>
+    <t xml:space="preserve">SERVO 0 CTL</t>
+  </si>
+  <si>
     <t xml:space="preserve">PB1</t>
   </si>
   <si>
@@ -191,6 +212,9 @@
     <t xml:space="preserve">TIM1_CH3N</t>
   </si>
   <si>
+    <t xml:space="preserve">SERVO 1 CTL</t>
+  </si>
+  <si>
     <t xml:space="preserve">PB2</t>
   </si>
   <si>
@@ -221,6 +245,9 @@
     <t xml:space="preserve">TIM3_CH1/PB4/SPI1_MISO</t>
   </si>
   <si>
+    <t xml:space="preserve">SERVO ENABLE</t>
+  </si>
+  <si>
     <t xml:space="preserve">PB5</t>
   </si>
   <si>
@@ -230,6 +257,9 @@
     <t xml:space="preserve">TIM3_CH2/SPI1_MOSI</t>
   </si>
   <si>
+    <t xml:space="preserve">MOTOR CTL A</t>
+  </si>
+  <si>
     <t xml:space="preserve">PB6</t>
   </si>
   <si>
@@ -239,6 +269,9 @@
     <t xml:space="preserve">USART1_TX</t>
   </si>
   <si>
+    <t xml:space="preserve">MOTOR CTL B</t>
+  </si>
+  <si>
     <t xml:space="preserve">PB7</t>
   </si>
   <si>
@@ -246,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">USART1_RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMOKE CTL</t>
   </si>
   <si>
     <t xml:space="preserve">PB8</t>
@@ -457,7 +493,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -506,381 +542,417 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>